<commit_message>
updated single child outputs
</commit_message>
<xml_diff>
--- a/outputs-HGR-r202/test-c__Elusimicrobia_split_pruned.xlsx
+++ b/outputs-HGR-r202/test-c__Elusimicrobia_split_pruned.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Row</t>
   </si>
@@ -52,7 +52,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -62,22 +62,14 @@
     </border>
     <border/>
     <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -96,18 +88,18 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -118,7 +110,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -129,7 +121,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4">

</xml_diff>